<commit_message>
complete manhour function: complete delete,search
</commit_message>
<xml_diff>
--- a/MH_NRC_Report_2023_08_05_12_23_45.xlsx
+++ b/MH_NRC_Report_2023_08_05_12_23_45.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="NRC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="91">
   <si>
     <t>NRC_ID</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>NRC</t>
+  </si>
+  <si>
+    <t>QZL0071</t>
   </si>
 </sst>
 </file>
@@ -690,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +832,7 @@
         <v>43</v>
       </c>
       <c r="J4">
-        <v>0.01</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -899,7 +902,7 @@
         <v>43</v>
       </c>
       <c r="J6">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="K6">
         <v>1.99</v>
@@ -973,6 +976,41 @@
       </c>
       <c r="K8">
         <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
complete nrc report detail and subtask win
</commit_message>
<xml_diff>
--- a/MH_NRC_Report_2023_08_05_12_23_45.xlsx
+++ b/MH_NRC_Report_2023_08_05_12_23_45.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V083COH\My_document\01_Work\30_Python_Projects\PTSS_3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="22368" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="NRC" sheetId="1" r:id="rId1"/>
     <sheet name="Subtask" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -58,100 +53,103 @@
     <t>QZL0010</t>
   </si>
   <si>
+    <t>B-HNU</t>
+  </si>
+  <si>
+    <t>777-BM-CONTROL-CARD-01</t>
+  </si>
+  <si>
+    <t>TOWING A/C FOR MAINTENANCE/OPERATIONAL NEEDS</t>
+  </si>
+  <si>
+    <t>FUS</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>QZL0028</t>
   </si>
   <si>
+    <t>AS PER B-HNU E-TECH LOG OPEN TL ENTRIES TL4332 - MSG APPEARED WHEN RIGHT WX SYS SELECTED.</t>
+  </si>
+  <si>
+    <t>CAB</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
     <t>QZL0036</t>
   </si>
   <si>
+    <t>777-5000-10-025-01</t>
+  </si>
+  <si>
+    <t>PLS REMOVE PED 1 2 4 5 HINGE COVER FOR EPAS BATTERIES REMOVE</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>5212</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
     <t>QZL0044</t>
   </si>
   <si>
+    <t>777-5000-10-026-01-1</t>
+  </si>
+  <si>
+    <t>AIRCRAFT REFUEL FOR PARKING</t>
+  </si>
+  <si>
+    <t>F/T</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
     <t>QZL0051</t>
   </si>
   <si>
+    <t>SWC-28778-01-01</t>
+  </si>
+  <si>
+    <t>ZONE B SEATS 39F 40B 43C 45A 39D 46A 48A 48B 50A 50B 50C 52A 52C 52F 49D 48E 47D 47E 46D 45F 44D 44E 41D 41F 40K 43J 43K 44H 45K 46H 46K 47H 47K 50H 50J 50K 51J 51K 52J 52K MONITOR TOUCHSCREEN FOUND MALFUNCTION</t>
+  </si>
+  <si>
+    <t>2332</t>
+  </si>
+  <si>
     <t>QZL0069</t>
   </si>
   <si>
+    <t>ZONE C SEAT 56B 57C 59A 59B 61A 61B 65C 66B 67B 66D 64D 64F 63D 62F 62D 61F 59F 57E 57G 56E 54G 55K 56J 59H 59J 61J 61H 62H64H 64K MONITOR TOUCHSCREEN FOUND MALFUNCTION</t>
+  </si>
+  <si>
     <t>QZL0070</t>
   </si>
   <si>
-    <t>B-HNU</t>
-  </si>
-  <si>
-    <t>777-BM-CONTROL-CARD-01</t>
-  </si>
-  <si>
-    <t>777-5000-10-025-01</t>
-  </si>
-  <si>
-    <t>777-5000-10-026-01-1</t>
-  </si>
-  <si>
-    <t>SWC-28778-01-01</t>
-  </si>
-  <si>
-    <t>TOWING A/C FOR MAINTENANCE/OPERATIONAL NEEDS</t>
-  </si>
-  <si>
-    <t>AS PER B-HNU E-TECH LOG OPEN TL ENTRIES TL4332 - MSG APPEARED WHEN RIGHT WX SYS SELECTED.</t>
-  </si>
-  <si>
-    <t>PLS REMOVE PED 1 2 4 5 HINGE COVER FOR EPAS BATTERIES REMOVE</t>
-  </si>
-  <si>
-    <t>AIRCRAFT REFUEL FOR PARKING</t>
-  </si>
-  <si>
-    <t>ZONE B SEATS 39F 40B 43C 45A 39D 46A 48A 48B 50A 50B 50C 52A 52C 52F 49D 48E 47D 47E 46D 45F 44D 44E 41D 41F 40K 43J 43K 44H 45K 46H 46K 47H 47K 50H 50J 50K 51J 51K 52J 52K MONITOR TOUCHSCREEN FOUND MALFUNCTION</t>
-  </si>
-  <si>
-    <t>ZONE C SEAT 56B 57C 59A 59B 61A 61B 65C 66B 67B 66D 64D 64F 63D 62F 62D 61F 59F 57E 57G 56E 54G 55K 56J 59H 59J 61J 61H 62H64H 64K MONITOR TOUCHSCREEN FOUND MALFUNCTION</t>
-  </si>
-  <si>
-    <t>FUS</t>
-  </si>
-  <si>
-    <t>CAB</t>
-  </si>
-  <si>
-    <t>F/T</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>AV</t>
-  </si>
-  <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>5212</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>2332</t>
-  </si>
-  <si>
-    <t>WIP</t>
-  </si>
-  <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>COMP</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>QZL0071</t>
   </si>
   <si>
     <t>Proj_Id</t>
@@ -175,6 +173,9 @@
     <t>QZ</t>
   </si>
   <si>
+    <t>NRC</t>
+  </si>
+  <si>
     <t>1C</t>
   </si>
   <si>
@@ -287,36 +288,187 @@
   </si>
   <si>
     <t>L007</t>
-  </si>
-  <si>
-    <t>NRC</t>
-  </si>
-  <si>
-    <t>QZL0071</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +481,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -377,9 +715,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -390,17 +970,61 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -449,7 +1073,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,7 +1108,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -687,21 +1311,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,33 +1360,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>43</v>
       </c>
       <c r="J2">
         <v>50.01</v>
@@ -771,30 +1395,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -803,33 +1427,33 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>4</v>
@@ -838,33 +1462,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -873,103 +1497,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J6">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="K6">
         <v>1.99</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>80</v>
+      </c>
+      <c r="K7">
+        <v>-20.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="I7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7">
-        <v>60</v>
-      </c>
-      <c r="K7">
-        <v>-20.010000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J8">
         <v>50</v>
@@ -978,33 +1602,33 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J9">
         <v>12</v>
@@ -1015,605 +1639,608 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.28703703703704" customWidth="1"/>
+    <col min="6" max="6" width="49.5740740740741" customWidth="1"/>
+    <col min="9" max="9" width="9.13888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="H3" s="4">
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H4" s="4">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H5" s="4">
         <v>5</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H6" s="4">
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H7" s="4">
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H10" s="4">
         <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H11" s="4">
         <v>5</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H12" s="4">
         <v>8</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="H13" s="4">
         <v>40</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H14" s="4">
         <v>48</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H15" s="4">
         <v>10</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H16" s="4">
         <v>6</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H17" s="4">
         <v>30</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H18" s="4">
         <v>36</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H19" s="4">
         <v>8</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H20" s="4">
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>